<commit_message>
Màj des stats. Prochaine eval3 : plus de poids sur le contrôle des tours !
</commit_message>
<xml_diff>
--- a/evals.xlsx
+++ b/evals.xlsx
@@ -435,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I10"/>
+  <dimension ref="C3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -470,8 +470,11 @@
       <c r="I4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="3">
         <v>0</v>
       </c>
@@ -481,8 +484,9 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>1</v>
       </c>
@@ -494,8 +498,9 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -509,16 +514,27 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -531,14 +547,38 @@
       <c r="F9">
         <v>4</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>5</v>
       </c>
       <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="J11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Erreurs corrigées + stats à refaire (parfois) +  eval5 fonctionnelle.
</commit_message>
<xml_diff>
--- a/evals.xlsx
+++ b/evals.xlsx
@@ -435,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J11"/>
+  <dimension ref="C3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -473,8 +473,11 @@
       <c r="J4">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="3">
         <v>0</v>
       </c>
@@ -485,8 +488,9 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
         <v>1</v>
       </c>
@@ -499,8 +503,9 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -515,8 +520,9 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -533,8 +539,9 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -553,15 +560,17 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>5</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>32</v>
       </c>
@@ -579,6 +588,18 @@
         <v>3</v>
       </c>
       <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Erreur orthographique dérangeante sur l'interface graphique
</commit_message>
<xml_diff>
--- a/evals.xlsx
+++ b/evals.xlsx
@@ -16,22 +16,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Gains pour les blancs (pertes pour les noirs) sur 5 parties</t>
   </si>
   <si>
     <t>EVAL N\B</t>
   </si>
+  <si>
+    <t>Gains pour les noirs maintenant /5 parties</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -134,6 +144,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +450,7 @@
   <dimension ref="C3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +459,9 @@
       <c r="D3" t="s">
         <v>0</v>
       </c>
+      <c r="I3" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
@@ -482,13 +497,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="3">
@@ -498,12 +513,12 @@
         <v>5</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
@@ -516,11 +531,11 @@
         <v>0</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
@@ -536,10 +551,10 @@
         <v>3</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="3">
@@ -558,17 +573,17 @@
         <v>1</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>5</v>
       </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -588,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -603,6 +618,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>